<commit_message>
Added Competition Types to the REST interface
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>35.5</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -552,10 +552,16 @@
       <c r="B15" s="2">
         <v>42958</v>
       </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>42961</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Competition to the REST interface
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>48.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -561,85 +561,88 @@
         <v>42961</v>
       </c>
       <c r="D16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>42962</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>42963</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>42964</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>42965</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>42968</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>42969</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>42970</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>42971</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>42972</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>42975</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>42976</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>42977</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>42978</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>42979</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>42982</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>42983</v>
       </c>

</xml_diff>

<commit_message>
Added Submissions + more Postman tests
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>57.5</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -575,6 +575,9 @@
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>42963</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Foreign keys to database
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -439,7 +439,7 @@
   <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>65.5</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -583,6 +583,9 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>42964</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some bugs with JSON
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>78.5</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -604,6 +604,9 @@
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>42969</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added MAven Project to EvaluationClient
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>86.5</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -612,6 +612,9 @@
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>42970</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added REST code to match REST documentation
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>94.5</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -620,6 +620,9 @@
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>42971</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Chaged organization of Eval Client a bit
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D33)</f>
-        <v>106.5</v>
+        <v>116.5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -652,6 +652,9 @@
       <c r="B29" s="2">
         <v>42978</v>
       </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
@@ -666,6 +669,9 @@
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>42983</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started client side javascript
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F3">
         <f>SUM(D3:D77)</f>
-        <v>136</v>
+        <v>139.75</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -723,6 +723,9 @@
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>42997</v>
+      </c>
+      <c r="D42">
+        <v>3.75</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated code added api functions
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -166,8 +166,8 @@
   </sheetPr>
   <dimension ref="B1:F77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -205,7 +205,7 @@
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">SUM(D3:D112)</f>
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,19 +620,22 @@
       <c r="B70" s="4" t="n">
         <v>43035</v>
       </c>
+      <c r="D70" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="4" t="n">
         <v>43040</v>
       </c>
-      <c r="D71" s="0" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="4" t="n">
         <v>43041</v>
       </c>
+      <c r="D72" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="4" t="n">
@@ -647,6 +650,9 @@
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="4" t="n">
         <v>43046</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed Bugs, added Team page
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -164,10 +164,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F80"/>
+  <dimension ref="B1:F82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E78" activeCellId="0" sqref="E78"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F80" activeCellId="0" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -205,7 +205,7 @@
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">SUM(D3:D150)</f>
-        <v>177.5</v>
+        <v>182.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,6 +669,11 @@
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D80" s="0" t="n">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D82" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished basic toggle functionality
</commit_message>
<xml_diff>
--- a/Docs/TimeLog.xlsx
+++ b/Docs/TimeLog.xlsx
@@ -164,9 +164,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F86"/>
+  <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G82" activeCellId="0" sqref="G82"/>
     </sheetView>
   </sheetViews>
@@ -205,7 +205,7 @@
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">SUM(D3:D150)</f>
-        <v>187.5</v>
+        <v>197.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,8 +676,18 @@
         <v>5</v>
       </c>
     </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D84" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D86" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D89" s="0" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>